<commit_message>
2.12 - lens fields
</commit_message>
<xml_diff>
--- a/documentation/Trian-gr - Σημεία ελέγχου.xlsx
+++ b/documentation/Trian-gr - Σημεία ελέγχου.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Trian\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA8CDCD-62CA-497A-8C4E-02A3CF6B5F5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114DC83B-2360-46EC-B32C-3E8B14173247}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Τα δεδομένα από το SoftOne παραλαμβάνονται και μπορούν να διαβαστούν</t>
   </si>
   <si>
-    <t>Ρύθμιση DNS Servers ώστε το (άδιεο) WordPress site να είναι online στη διέυθυνση trian.gr, με χρήση SSL.</t>
-  </si>
-  <si>
     <t>Σχεδιασμός αρχιτεκτονικής ροής δεδομένων</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>TRIAN.GR</t>
+  </si>
+  <si>
+    <t>Ρύθμιση DNS Servers ώστε το (άδειο) WordPress site να είναι online στη διέυθυνση trian.gr, με χρήση SSL.</t>
   </si>
 </sst>
 </file>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -514,7 +514,7 @@
     </row>
     <row r="4" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -522,7 +522,7 @@
     </row>
     <row r="5" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -530,7 +530,7 @@
     </row>
     <row r="6" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -538,7 +538,7 @@
     </row>
     <row r="7" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -546,7 +546,7 @@
     </row>
     <row r="8" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="9" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -562,7 +562,7 @@
     </row>
     <row r="10" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -570,7 +570,7 @@
     </row>
     <row r="11" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -578,7 +578,7 @@
     </row>
     <row r="12" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -586,7 +586,7 @@
     </row>
     <row r="13" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -594,7 +594,7 @@
     </row>
     <row r="14" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -602,7 +602,7 @@
     </row>
     <row r="15" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -610,7 +610,7 @@
     </row>
     <row r="16" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -618,7 +618,7 @@
     </row>
     <row r="17" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -626,7 +626,7 @@
     </row>
     <row r="18" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -634,7 +634,7 @@
     </row>
     <row r="19" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -642,7 +642,7 @@
     </row>
     <row r="20" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>

</xml_diff>